<commit_message>
Completed all data preprocessing. April 25, 2018
</commit_message>
<xml_diff>
--- a/query_Accession_results.xlsx
+++ b/query_Accession_results.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="187">
   <si>
     <t xml:space="preserve">uid</t>
   </si>
@@ -29,498 +29,507 @@
     <t xml:space="preserve">start.pos</t>
   </si>
   <si>
-    <t xml:space="preserve">RNA28SN5</t>
+    <t xml:space="preserve">143188</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC143188</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">155060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC155060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">158318</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAM27E1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">283874</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC283874</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">284009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC284009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">339457</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1orf222</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">340843</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAM23B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">387720</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC387720</t>
+  </si>
+  <si>
+    <t xml:space="preserve">387790</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC387790</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">387820</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC387820</t>
+  </si>
+  <si>
+    <t xml:space="preserve">388022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC388022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">392395</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC392395</t>
+  </si>
+  <si>
+    <t xml:space="preserve">400499</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC400499</t>
+  </si>
+  <si>
+    <t xml:space="preserve">400924</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC400924</t>
   </si>
   <si>
     <t xml:space="preserve">22</t>
   </si>
   <si>
-    <t xml:space="preserve">KLRA1P</t>
+    <t xml:space="preserve">401052</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC401052</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">401296</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LNCRI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">401410</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC401410</t>
+  </si>
+  <si>
+    <t xml:space="preserve">401433</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC401433</t>
+  </si>
+  <si>
+    <t xml:space="preserve">401589</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC401589</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">401620</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC401620</t>
+  </si>
+  <si>
+    <t xml:space="preserve">401622</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC401622</t>
+  </si>
+  <si>
+    <t xml:space="preserve">440570</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC440570</t>
+  </si>
+  <si>
+    <t xml:space="preserve">441120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC441120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">441136</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC441136</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">441179</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC441179</t>
+  </si>
+  <si>
+    <t xml:space="preserve">441193</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC441193</t>
+  </si>
+  <si>
+    <t xml:space="preserve">441233</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC441233</t>
+  </si>
+  <si>
+    <t xml:space="preserve">441257</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC441257</t>
+  </si>
+  <si>
+    <t xml:space="preserve">441956</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC441956</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">541473</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC541473</t>
+  </si>
+  <si>
+    <t xml:space="preserve">643576</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC643576</t>
   </si>
   <si>
     <t xml:space="preserve">12</t>
   </si>
   <si>
-    <t xml:space="preserve">ALS2CR16</t>
+    <t xml:space="preserve">644563</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC644563</t>
+  </si>
+  <si>
+    <t xml:space="preserve">646347</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC646347</t>
+  </si>
+  <si>
+    <t xml:space="preserve">646434</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC646434</t>
+  </si>
+  <si>
+    <t xml:space="preserve">646517</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC646517</t>
+  </si>
+  <si>
+    <t xml:space="preserve">653365</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASAH2C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">653501</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC653501</t>
+  </si>
+  <si>
+    <t xml:space="preserve">727726</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC727726</t>
+  </si>
+  <si>
+    <t xml:space="preserve">727797</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC727797</t>
+  </si>
+  <si>
+    <t xml:space="preserve">727849</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC727849</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">728392</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC728392</t>
+  </si>
+  <si>
+    <t xml:space="preserve">728454</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEFB4B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">728554</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC728554</t>
+  </si>
+  <si>
+    <t xml:space="preserve">729021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC729021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88523</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC88523</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">91431</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC91431</t>
+  </si>
+  <si>
+    <t xml:space="preserve">93622</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC93622</t>
+  </si>
+  <si>
+    <t xml:space="preserve">115648</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC115648</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">285074</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC285074</t>
   </si>
   <si>
     <t xml:space="preserve">2</t>
   </si>
   <si>
-    <t xml:space="preserve">C12orf63</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GUSBP4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC387820</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC392395</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LINC00999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RASA4CP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RPS2P8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC441956</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21</t>
+    <t xml:space="preserve">286526</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAR2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">389833</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC389833</t>
+  </si>
+  <si>
+    <t xml:space="preserve">389834</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC389834</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un</t>
+  </si>
+  <si>
+    <t xml:space="preserve">400464</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC400464</t>
+  </si>
+  <si>
+    <t xml:space="preserve">400968</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC400968</t>
+  </si>
+  <si>
+    <t xml:space="preserve">401252</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC401252</t>
+  </si>
+  <si>
+    <t xml:space="preserve">440337</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC440337</t>
+  </si>
+  <si>
+    <t xml:space="preserve">440568</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC440568</t>
+  </si>
+  <si>
+    <t xml:space="preserve">441070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC441070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">441268</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC441268</t>
+  </si>
+  <si>
+    <t xml:space="preserve">442535</t>
   </si>
   <si>
     <t xml:space="preserve">LOC442535</t>
   </si>
   <si>
-    <t xml:space="preserve">PMS2P2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FAM45BP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPANXB2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SNHG3-RCC1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SYS1-DBNDD2</t>
+    <t xml:space="preserve">541469</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC541469</t>
+  </si>
+  <si>
+    <t xml:space="preserve">642897</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC642897</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90925</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC90925</t>
+  </si>
+  <si>
+    <t xml:space="preserve">143666</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC143666</t>
+  </si>
+  <si>
+    <t xml:space="preserve">284296</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC284296</t>
+  </si>
+  <si>
+    <t xml:space="preserve">400965</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC400965</t>
+  </si>
+  <si>
+    <t xml:space="preserve">401072</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC401072</t>
+  </si>
+  <si>
+    <t xml:space="preserve">402110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC402110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">439985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC439985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">440742</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC440742</t>
+  </si>
+  <si>
+    <t xml:space="preserve">613266</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC613266</t>
   </si>
   <si>
     <t xml:space="preserve">20</t>
   </si>
   <si>
-    <t xml:space="preserve">LINC00341</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BIN3-IT1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC90925</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC93622</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">115648</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC115648</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">155060</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC155060</t>
-  </si>
-  <si>
-    <t xml:space="preserve">283874</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC283874</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">285074</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC285074</t>
-  </si>
-  <si>
-    <t xml:space="preserve">286526</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RAR2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">339457</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C1orf222</t>
-  </si>
-  <si>
-    <t xml:space="preserve">387820</t>
-  </si>
-  <si>
-    <t xml:space="preserve">388022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC388022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">389833</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC389833</t>
-  </si>
-  <si>
-    <t xml:space="preserve">389834</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC389834</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Un</t>
-  </si>
-  <si>
-    <t xml:space="preserve">400464</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC400464</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">400499</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC400499</t>
-  </si>
-  <si>
-    <t xml:space="preserve">400924</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC400924</t>
-  </si>
-  <si>
-    <t xml:space="preserve">400968</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC400968</t>
-  </si>
-  <si>
-    <t xml:space="preserve">401252</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC401252</t>
-  </si>
-  <si>
-    <t xml:space="preserve">401589</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC401589</t>
-  </si>
-  <si>
-    <t xml:space="preserve">440337</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC440337</t>
-  </si>
-  <si>
-    <t xml:space="preserve">440568</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC440568</t>
-  </si>
-  <si>
-    <t xml:space="preserve">440570</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC440570</t>
-  </si>
-  <si>
-    <t xml:space="preserve">441070</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC441070</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">441120</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC441120</t>
-  </si>
-  <si>
-    <t xml:space="preserve">441193</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC441193</t>
-  </si>
-  <si>
-    <t xml:space="preserve">441257</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC441257</t>
-  </si>
-  <si>
-    <t xml:space="preserve">441268</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC441268</t>
-  </si>
-  <si>
-    <t xml:space="preserve">441956</t>
-  </si>
-  <si>
-    <t xml:space="preserve">442535</t>
-  </si>
-  <si>
-    <t xml:space="preserve">541469</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC541469</t>
-  </si>
-  <si>
-    <t xml:space="preserve">541473</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC541473</t>
-  </si>
-  <si>
-    <t xml:space="preserve">642897</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC642897</t>
-  </si>
-  <si>
-    <t xml:space="preserve">643576</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC643576</t>
-  </si>
-  <si>
-    <t xml:space="preserve">644563</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC644563</t>
-  </si>
-  <si>
-    <t xml:space="preserve">646347</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC646347</t>
-  </si>
-  <si>
-    <t xml:space="preserve">646517</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC646517</t>
-  </si>
-  <si>
-    <t xml:space="preserve">727726</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC727726</t>
-  </si>
-  <si>
-    <t xml:space="preserve">727849</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC727849</t>
-  </si>
-  <si>
-    <t xml:space="preserve">728392</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC728392</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">728454</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEFB4B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">88523</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC88523</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">90925</t>
-  </si>
-  <si>
-    <t xml:space="preserve">91431</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC91431</t>
-  </si>
-  <si>
-    <t xml:space="preserve">143188</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC143188</t>
-  </si>
-  <si>
-    <t xml:space="preserve">143666</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC143666</t>
-  </si>
-  <si>
-    <t xml:space="preserve">284009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC284009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">284296</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC284296</t>
-  </si>
-  <si>
-    <t xml:space="preserve">340843</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FAM23B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">387720</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC387720</t>
-  </si>
-  <si>
-    <t xml:space="preserve">387790</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC387790</t>
-  </si>
-  <si>
-    <t xml:space="preserve">392395</t>
-  </si>
-  <si>
-    <t xml:space="preserve">400965</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC400965</t>
-  </si>
-  <si>
-    <t xml:space="preserve">401052</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC401052</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">401072</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC401072</t>
-  </si>
-  <si>
-    <t xml:space="preserve">401410</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC401410</t>
-  </si>
-  <si>
-    <t xml:space="preserve">402110</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC402110</t>
-  </si>
-  <si>
-    <t xml:space="preserve">439985</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC439985</t>
-  </si>
-  <si>
-    <t xml:space="preserve">440742</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC440742</t>
-  </si>
-  <si>
-    <t xml:space="preserve">441233</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC441233</t>
-  </si>
-  <si>
-    <t xml:space="preserve">613266</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC613266</t>
-  </si>
-  <si>
-    <t xml:space="preserve">646434</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC646434</t>
-  </si>
-  <si>
     <t xml:space="preserve">647115</t>
   </si>
   <si>
     <t xml:space="preserve">LOC647115</t>
   </si>
   <si>
-    <t xml:space="preserve">727797</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC727797</t>
-  </si>
-  <si>
-    <t xml:space="preserve">729021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC729021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">93622</t>
-  </si>
-  <si>
-    <t xml:space="preserve">158318</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FAM27E1</t>
-  </si>
-  <si>
     <t xml:space="preserve">284912</t>
   </si>
   <si>
@@ -545,30 +554,12 @@
     <t xml:space="preserve">LOC399900</t>
   </si>
   <si>
-    <t xml:space="preserve">401296</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LNCRI</t>
-  </si>
-  <si>
     <t xml:space="preserve">401357</t>
   </si>
   <si>
     <t xml:space="preserve">LOC401357</t>
   </si>
   <si>
-    <t xml:space="preserve">401433</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC401433</t>
-  </si>
-  <si>
-    <t xml:space="preserve">401620</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC401620</t>
-  </si>
-  <si>
     <t xml:space="preserve">440258</t>
   </si>
   <si>
@@ -579,12 +570,6 @@
   </si>
   <si>
     <t xml:space="preserve">FAM27E2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">653365</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASAH2C</t>
   </si>
   <si>
     <t xml:space="preserve">94431</t>
@@ -638,8 +623,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:D22" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:D22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:D48" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:D48"/>
   <tableColumns count="4">
     <tableColumn id="1" name="uid"/>
     <tableColumn id="2" name="name"/>
@@ -989,280 +974,624 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>100008589</v>
+      <c r="A2" t="s">
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2"/>
+        <v>6</v>
+      </c>
+      <c r="D2" t="n">
+        <v>114.610672</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>10748</v>
+      <c r="A3" t="s">
+        <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="n">
+        <v>149.28528</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2.65115</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2.40698</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="n">
-        <v>10.588477</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>130029</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D8" t="n">
+        <v>18.081223</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="n">
+        <v>127.734609</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="n">
+        <v>127.940983</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="n">
+        <v>104.719759</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" t="n">
+        <v>11.372014</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" t="n">
+        <v>10.006417</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="n">
-        <v>203.559077</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>374467</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>375513</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D17" t="n">
+        <v>1.690811</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" t="n">
+        <v>151.07413</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" t="n">
+        <v>52.05117</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" t="n">
+        <v>167.795528</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" t="n">
+        <v>5.426139</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" t="n">
+        <v>57.475796</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" t="n">
+        <v>13.679218</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" t="n">
+        <v>75.391948</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" t="n">
+        <v>104.030728</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" t="n">
+        <v>107.131573</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>83</v>
+      </c>
+      <c r="B34" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" t="n">
+        <v>160.894888</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" t="n">
+        <v>51.409883</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>89</v>
+      </c>
+      <c r="B37" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" t="n">
+        <v>50.187239</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" t="s">
+        <v>92</v>
+      </c>
+      <c r="C38" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="n">
-        <v>57.908552</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>387820</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="n">
-        <v>127.940983</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>392395</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>399744</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D38" t="n">
+        <v>39.443813</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" t="n">
+        <v>50.69633</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>95</v>
+      </c>
+      <c r="B40" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" t="s">
+        <v>43</v>
+      </c>
+      <c r="D40"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>97</v>
+      </c>
+      <c r="B41" t="s">
+        <v>98</v>
+      </c>
+      <c r="C41" t="s">
+        <v>99</v>
+      </c>
+      <c r="D41"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>100</v>
+      </c>
+      <c r="B42" t="s">
+        <v>101</v>
+      </c>
+      <c r="C42" t="s">
         <v>18</v>
       </c>
-      <c r="D9" t="n">
-        <v>38.428145</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>401331</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" t="n">
-        <v>44.028886</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>440589</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" t="n">
-        <v>51.250561</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>441956</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" t="n">
-        <v>13.679218</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>442535</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>5380</v>
-      </c>
-      <c r="B14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" t="n">
-        <v>75.343936</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>55855</v>
-      </c>
-      <c r="B15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" t="n">
-        <v>130.49494</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>64694</v>
-      </c>
-      <c r="B16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>751867</v>
-      </c>
-      <c r="B17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17"/>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>767557</v>
-      </c>
-      <c r="B18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" t="n">
-        <v>45.363168</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>79686</v>
-      </c>
-      <c r="B19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19"/>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>80094</v>
-      </c>
-      <c r="B20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" t="n">
-        <v>22.64037</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>90925</v>
-      </c>
-      <c r="B21" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21"/>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>93622</v>
-      </c>
-      <c r="B22" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" t="n">
+      <c r="D42" t="n">
+        <v>5.499426</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>102</v>
+      </c>
+      <c r="B43" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" t="n">
+        <v>7.259787</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>105</v>
+      </c>
+      <c r="B44" t="s">
+        <v>106</v>
+      </c>
+      <c r="C44" t="s">
+        <v>61</v>
+      </c>
+      <c r="D44" t="n">
+        <v>177.87526</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>107</v>
+      </c>
+      <c r="B45" t="s">
+        <v>108</v>
+      </c>
+      <c r="C45" t="s">
+        <v>109</v>
+      </c>
+      <c r="D45"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>110</v>
+      </c>
+      <c r="B46" t="s">
+        <v>111</v>
+      </c>
+      <c r="C46" t="s">
+        <v>112</v>
+      </c>
+      <c r="D46"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>113</v>
+      </c>
+      <c r="B47" t="s">
+        <v>114</v>
+      </c>
+      <c r="C47" t="s">
+        <v>109</v>
+      </c>
+      <c r="D47"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>115</v>
+      </c>
+      <c r="B48" t="s">
+        <v>116</v>
+      </c>
+      <c r="C48" t="s">
+        <v>109</v>
+      </c>
+      <c r="D48" t="n">
         <v>6.674093</v>
       </c>
     </row>
@@ -1299,25 +1628,25 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>119</v>
       </c>
       <c r="D2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D3" t="n">
         <v>149.28528</v>
@@ -1325,13 +1654,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="D4" t="n">
         <v>2.65115</v>
@@ -1339,13 +1668,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>120</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>121</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>122</v>
       </c>
       <c r="D5" t="n">
         <v>87.030674</v>
@@ -1353,37 +1682,37 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>123</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>124</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D8" t="n">
         <v>127.940983</v>
@@ -1391,13 +1720,13 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" t="n">
         <v>104.719759</v>
@@ -1405,37 +1734,37 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>125</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>126</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="D10"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>127</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>128</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>129</v>
       </c>
       <c r="D11"/>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>130</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>131</v>
       </c>
       <c r="C12" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="D12" t="n">
         <v>99.807022</v>
@@ -1443,13 +1772,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="D13" t="n">
         <v>11.372014</v>
@@ -1457,25 +1786,25 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="D14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>69</v>
+        <v>132</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>133</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="D15" t="n">
         <v>19.62067</v>
@@ -1483,13 +1812,13 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>134</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>135</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="D16" t="n">
         <v>32.331465</v>
@@ -1497,13 +1826,13 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D17" t="n">
         <v>52.05117</v>
@@ -1511,13 +1840,13 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>136</v>
       </c>
       <c r="B18" t="s">
-        <v>76</v>
+        <v>137</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="D18" t="n">
         <v>6.377742</v>
@@ -1525,13 +1854,13 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>77</v>
+        <v>138</v>
       </c>
       <c r="B19" t="s">
-        <v>78</v>
+        <v>139</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D19" t="n">
         <v>16.034509</v>
@@ -1539,25 +1868,25 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D20"/>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>81</v>
+        <v>140</v>
       </c>
       <c r="B21" t="s">
-        <v>82</v>
+        <v>141</v>
       </c>
       <c r="C21" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D21" t="n">
         <v>44.874939</v>
@@ -1565,25 +1894,25 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="C22" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D22"/>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D23" t="n">
         <v>5.426139</v>
@@ -1591,37 +1920,37 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="C24" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D24"/>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>90</v>
+        <v>142</v>
       </c>
       <c r="B25" t="s">
-        <v>91</v>
+        <v>143</v>
       </c>
       <c r="C25" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D25"/>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="C26" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="D26" t="n">
         <v>13.679218</v>
@@ -1629,37 +1958,37 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>93</v>
+        <v>144</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>145</v>
       </c>
       <c r="C27" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D27"/>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>146</v>
       </c>
       <c r="B28" t="s">
-        <v>95</v>
+        <v>147</v>
       </c>
       <c r="C28" t="s">
-        <v>42</v>
+        <v>119</v>
       </c>
       <c r="D28"/>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="B29" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="C29" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D29" t="n">
         <v>75.391948</v>
@@ -1667,13 +1996,13 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>98</v>
+        <v>148</v>
       </c>
       <c r="B30" t="s">
-        <v>99</v>
+        <v>149</v>
       </c>
       <c r="C30" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D30" t="n">
         <v>93.609431</v>
@@ -1681,13 +2010,13 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="B31" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>7</v>
+        <v>80</v>
       </c>
       <c r="D31" t="n">
         <v>104.030728</v>
@@ -1695,13 +2024,13 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="B32" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="C32" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D32" t="n">
         <v>107.131573</v>
@@ -1709,13 +2038,13 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="B33" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="C33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D33" t="n">
         <v>160.894888</v>
@@ -1723,13 +2052,13 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="B34" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="C34" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="D34" t="n">
         <v>51.409883</v>
@@ -1737,13 +2066,13 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="B35" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="C35" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D35" t="n">
         <v>50.69633</v>
@@ -1751,25 +2080,25 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="B36" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C36" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="D36"/>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B37" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C37" t="s">
-        <v>114</v>
+        <v>18</v>
       </c>
       <c r="D37" t="n">
         <v>5.499426</v>
@@ -1777,13 +2106,13 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="B38" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C38" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="D38" t="n">
         <v>7.259787</v>
@@ -1791,37 +2120,37 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B39" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C39" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D39"/>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="B40" t="s">
-        <v>37</v>
+        <v>151</v>
       </c>
       <c r="C40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D40"/>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B41" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C41" t="s">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="D41"/>
     </row>
@@ -1858,25 +2187,25 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>119</v>
       </c>
       <c r="D2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>124</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D3" t="n">
         <v>114.610672</v>
@@ -1884,13 +2213,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>152</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>153</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D4" t="n">
         <v>0.573807</v>
@@ -1898,13 +2227,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="D5" t="n">
         <v>2.65115</v>
@@ -1912,13 +2241,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>114</v>
+        <v>18</v>
       </c>
       <c r="D6" t="n">
         <v>2.40698</v>
@@ -1926,25 +2255,25 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
       <c r="B7" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>119</v>
       </c>
       <c r="D7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>120</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>121</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>122</v>
       </c>
       <c r="D8" t="n">
         <v>87.030674</v>
@@ -1952,25 +2281,25 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>123</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>124</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D9"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>132</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D10" t="n">
         <v>18.081223</v>
@@ -1978,13 +2307,13 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>133</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>134</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D11" t="n">
         <v>127.734609</v>
@@ -1992,25 +2321,25 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>135</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>136</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D12"/>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D13" t="n">
         <v>127.940983</v>
@@ -2018,13 +2347,13 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" t="n">
         <v>104.719759</v>
@@ -2032,37 +2361,37 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>125</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>126</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="D15"/>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>137</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D16"/>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>130</v>
       </c>
       <c r="B17" t="s">
-        <v>63</v>
+        <v>131</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="D17" t="n">
         <v>99.807022</v>
@@ -2070,13 +2399,13 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="D18" t="n">
         <v>11.372014</v>
@@ -2084,25 +2413,25 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="D19"/>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
       <c r="B20" t="s">
-        <v>139</v>
+        <v>157</v>
       </c>
       <c r="C20" t="s">
-        <v>9</v>
+        <v>122</v>
       </c>
       <c r="D20" t="n">
         <v>87.052748</v>
@@ -2110,13 +2439,13 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>140</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>141</v>
+        <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>142</v>
+        <v>43</v>
       </c>
       <c r="D21" t="n">
         <v>10.006417</v>
@@ -2124,13 +2453,13 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
       <c r="B22" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="C22" t="s">
-        <v>142</v>
+        <v>43</v>
       </c>
       <c r="D22" t="n">
         <v>70.745438</v>
@@ -2138,25 +2467,25 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>145</v>
+        <v>46</v>
       </c>
       <c r="B23" t="s">
-        <v>146</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D23"/>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D24" t="n">
         <v>52.05117</v>
@@ -2164,13 +2493,13 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="B25" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="C25" t="s">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="D25" t="n">
         <v>48.992527</v>
@@ -2178,13 +2507,13 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="B26" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C26" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D26" t="n">
         <v>76.825429</v>
@@ -2192,13 +2521,13 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>136</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>137</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="D27" t="n">
         <v>6.377742</v>
@@ -2206,13 +2535,13 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>77</v>
+        <v>138</v>
       </c>
       <c r="B28" t="s">
-        <v>78</v>
+        <v>139</v>
       </c>
       <c r="C28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D28" t="n">
         <v>16.034509</v>
@@ -2220,25 +2549,25 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="B29" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="C29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D29"/>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="B30" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="C30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D30" t="n">
         <v>244.064329</v>
@@ -2246,25 +2575,25 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="B31" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="C31" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>153</v>
+        <v>69</v>
       </c>
       <c r="B32" t="s">
-        <v>154</v>
+        <v>70</v>
       </c>
       <c r="C32" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D32" t="n">
         <v>57.475796</v>
@@ -2272,37 +2601,37 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="B33" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="C33" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D33"/>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>90</v>
+        <v>142</v>
       </c>
       <c r="B34" t="s">
-        <v>91</v>
+        <v>143</v>
       </c>
       <c r="C34" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D34"/>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="B35" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="C35" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="D35" t="n">
         <v>13.679218</v>
@@ -2310,25 +2639,25 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>94</v>
+        <v>146</v>
       </c>
       <c r="B36" t="s">
-        <v>95</v>
+        <v>147</v>
       </c>
       <c r="C36" t="s">
-        <v>42</v>
+        <v>119</v>
       </c>
       <c r="D36"/>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="B37" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="C37" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D37" t="n">
         <v>75.391948</v>
@@ -2336,13 +2665,13 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="B38" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="C38" t="s">
-        <v>32</v>
+        <v>168</v>
       </c>
       <c r="D38" t="n">
         <v>15.892332</v>
@@ -2350,13 +2679,13 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="B39" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="C39" t="s">
-        <v>7</v>
+        <v>80</v>
       </c>
       <c r="D39" t="n">
         <v>104.030728</v>
@@ -2364,13 +2693,13 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="B40" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="C40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D40" t="n">
         <v>160.894888</v>
@@ -2378,25 +2707,25 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>157</v>
+        <v>85</v>
       </c>
       <c r="B41" t="s">
-        <v>158</v>
+        <v>86</v>
       </c>
       <c r="C41" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D41"/>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="B42" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="C42" t="s">
-        <v>9</v>
+        <v>122</v>
       </c>
       <c r="D42" t="n">
         <v>63.841106</v>
@@ -2404,13 +2733,13 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="B43" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="C43" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D43" t="n">
         <v>50.69633</v>
@@ -2418,73 +2747,73 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>161</v>
+        <v>95</v>
       </c>
       <c r="B44" t="s">
-        <v>162</v>
+        <v>96</v>
       </c>
       <c r="C44" t="s">
-        <v>142</v>
+        <v>43</v>
       </c>
       <c r="D44"/>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="B45" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C45" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="D45"/>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>163</v>
+        <v>107</v>
       </c>
       <c r="B46" t="s">
-        <v>164</v>
+        <v>108</v>
       </c>
       <c r="C46" t="s">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="D46"/>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B47" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C47" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D47"/>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B48" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C48" t="s">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="D48"/>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>165</v>
+        <v>115</v>
       </c>
       <c r="B49" t="s">
-        <v>38</v>
+        <v>116</v>
       </c>
       <c r="C49" t="s">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="D49" t="n">
         <v>6.674093</v>
@@ -2523,25 +2852,25 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>119</v>
       </c>
       <c r="D2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>124</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D3" t="n">
         <v>114.610672</v>
@@ -2549,13 +2878,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>152</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>153</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D4" t="n">
         <v>0.573807</v>
@@ -2563,13 +2892,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D5" t="n">
         <v>149.28528</v>
@@ -2577,25 +2906,25 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>166</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>167</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="D7" t="n">
         <v>2.65115</v>
@@ -2603,13 +2932,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B8" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="D8" t="n">
         <v>35.627575</v>
@@ -2617,37 +2946,37 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>123</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>124</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D9"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D11" t="n">
         <v>127.940983</v>
@@ -2655,13 +2984,13 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B12" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="D12" t="n">
         <v>7.939</v>
@@ -2669,13 +2998,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B13" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D13" t="n">
         <v>72.490259</v>
@@ -2683,37 +3012,37 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>125</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>126</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="D14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>137</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D15"/>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B16" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C16" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D16" t="n">
         <v>61.967797</v>
@@ -2721,13 +3050,13 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="D17" t="n">
         <v>11.372014</v>
@@ -2735,13 +3064,13 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
       <c r="B18" t="s">
-        <v>139</v>
+        <v>157</v>
       </c>
       <c r="C18" t="s">
-        <v>9</v>
+        <v>122</v>
       </c>
       <c r="D18" t="n">
         <v>87.052748</v>
@@ -2749,13 +3078,13 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>140</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>141</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>142</v>
+        <v>43</v>
       </c>
       <c r="D19" t="n">
         <v>10.006417</v>
@@ -2763,13 +3092,13 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>134</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>135</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="D20" t="n">
         <v>32.331465</v>
@@ -2777,13 +3106,13 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>176</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>177</v>
+        <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D21" t="n">
         <v>1.690811</v>
@@ -2791,13 +3120,13 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B22" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D22" t="n">
         <v>56.809123</v>
@@ -2805,13 +3134,13 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>180</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>181</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D23" t="n">
         <v>151.07413</v>
@@ -2819,37 +3148,37 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>182</v>
+        <v>53</v>
       </c>
       <c r="B24" t="s">
-        <v>183</v>
+        <v>54</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D24"/>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B25" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="D25"/>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>136</v>
       </c>
       <c r="B26" t="s">
-        <v>76</v>
+        <v>137</v>
       </c>
       <c r="C26" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="D26" t="n">
         <v>6.377742</v>
@@ -2857,13 +3186,13 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>138</v>
       </c>
       <c r="B27" t="s">
-        <v>78</v>
+        <v>139</v>
       </c>
       <c r="C27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D27" t="n">
         <v>16.034509</v>
@@ -2871,37 +3200,37 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="B28" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="C28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D28"/>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="C29" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D29"/>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="B30" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="C30" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D30" t="n">
         <v>5.426139</v>
@@ -2909,25 +3238,25 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="B31" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="C31" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="B32" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="C32" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="D32" t="n">
         <v>13.679218</v>
@@ -2935,25 +3264,25 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B33" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C33" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D33"/>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="B34" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="C34" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D34" t="n">
         <v>75.391948</v>
@@ -2961,13 +3290,13 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="B35" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="C35" t="s">
-        <v>32</v>
+        <v>168</v>
       </c>
       <c r="D35" t="n">
         <v>15.892332</v>
@@ -2975,13 +3304,13 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="B36" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="C36" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D36" t="n">
         <v>107.131573</v>
@@ -2989,13 +3318,13 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="B37" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="C37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D37" t="n">
         <v>160.894888</v>
@@ -3003,25 +3332,25 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>157</v>
+        <v>85</v>
       </c>
       <c r="B38" t="s">
-        <v>158</v>
+        <v>86</v>
       </c>
       <c r="C38" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D38"/>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="B39" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="C39" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="D39" t="n">
         <v>51.409883</v>
@@ -3029,13 +3358,13 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="B40" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="C40" t="s">
-        <v>9</v>
+        <v>122</v>
       </c>
       <c r="D40" t="n">
         <v>63.841106</v>
@@ -3043,13 +3372,13 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>188</v>
+        <v>89</v>
       </c>
       <c r="B41" t="s">
-        <v>189</v>
+        <v>90</v>
       </c>
       <c r="C41" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D41" t="n">
         <v>50.187239</v>
@@ -3057,13 +3386,13 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="B42" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="C42" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D42" t="n">
         <v>50.69633</v>
@@ -3071,37 +3400,37 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>161</v>
+        <v>95</v>
       </c>
       <c r="B43" t="s">
-        <v>162</v>
+        <v>96</v>
       </c>
       <c r="C43" t="s">
-        <v>142</v>
+        <v>43</v>
       </c>
       <c r="D43"/>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="B44" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C44" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="D44"/>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B45" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C45" t="s">
-        <v>114</v>
+        <v>18</v>
       </c>
       <c r="D45" t="n">
         <v>5.499426</v>
@@ -3109,13 +3438,13 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="B46" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C46" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="D46" t="n">
         <v>7.259787</v>
@@ -3123,25 +3452,25 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="B47" t="s">
-        <v>37</v>
+        <v>151</v>
       </c>
       <c r="C47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D47"/>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B48" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C48" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="D48" t="n">
         <v>21.715451</v>

</xml_diff>

<commit_message>
rewound the commits back at least 5 steps.
</commit_message>
<xml_diff>
--- a/query_Accession_results.xlsx
+++ b/query_Accession_results.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="187">
   <si>
     <t xml:space="preserve">uid</t>
   </si>
@@ -29,498 +29,507 @@
     <t xml:space="preserve">start.pos</t>
   </si>
   <si>
-    <t xml:space="preserve">RNA28SN5</t>
+    <t xml:space="preserve">143188</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC143188</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">155060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC155060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">158318</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAM27E1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">283874</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC283874</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">284009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC284009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">339457</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1orf222</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">340843</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAM23B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">387720</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC387720</t>
+  </si>
+  <si>
+    <t xml:space="preserve">387790</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC387790</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">387820</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC387820</t>
+  </si>
+  <si>
+    <t xml:space="preserve">388022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC388022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">392395</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC392395</t>
+  </si>
+  <si>
+    <t xml:space="preserve">400499</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC400499</t>
+  </si>
+  <si>
+    <t xml:space="preserve">400924</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC400924</t>
   </si>
   <si>
     <t xml:space="preserve">22</t>
   </si>
   <si>
-    <t xml:space="preserve">KLRA1P</t>
+    <t xml:space="preserve">401052</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC401052</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">401296</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LNCRI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">401410</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC401410</t>
+  </si>
+  <si>
+    <t xml:space="preserve">401433</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC401433</t>
+  </si>
+  <si>
+    <t xml:space="preserve">401589</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC401589</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">401620</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC401620</t>
+  </si>
+  <si>
+    <t xml:space="preserve">401622</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC401622</t>
+  </si>
+  <si>
+    <t xml:space="preserve">440570</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC440570</t>
+  </si>
+  <si>
+    <t xml:space="preserve">441120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC441120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">441136</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC441136</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">441179</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC441179</t>
+  </si>
+  <si>
+    <t xml:space="preserve">441193</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC441193</t>
+  </si>
+  <si>
+    <t xml:space="preserve">441233</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC441233</t>
+  </si>
+  <si>
+    <t xml:space="preserve">441257</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC441257</t>
+  </si>
+  <si>
+    <t xml:space="preserve">441956</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC441956</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">541473</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC541473</t>
+  </si>
+  <si>
+    <t xml:space="preserve">643576</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC643576</t>
   </si>
   <si>
     <t xml:space="preserve">12</t>
   </si>
   <si>
-    <t xml:space="preserve">ALS2CR16</t>
+    <t xml:space="preserve">644563</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC644563</t>
+  </si>
+  <si>
+    <t xml:space="preserve">646347</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC646347</t>
+  </si>
+  <si>
+    <t xml:space="preserve">646434</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC646434</t>
+  </si>
+  <si>
+    <t xml:space="preserve">646517</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC646517</t>
+  </si>
+  <si>
+    <t xml:space="preserve">653365</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASAH2C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">653501</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC653501</t>
+  </si>
+  <si>
+    <t xml:space="preserve">727726</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC727726</t>
+  </si>
+  <si>
+    <t xml:space="preserve">727797</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC727797</t>
+  </si>
+  <si>
+    <t xml:space="preserve">727849</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC727849</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">728392</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC728392</t>
+  </si>
+  <si>
+    <t xml:space="preserve">728454</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEFB4B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">728554</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC728554</t>
+  </si>
+  <si>
+    <t xml:space="preserve">729021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC729021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88523</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC88523</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">91431</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC91431</t>
+  </si>
+  <si>
+    <t xml:space="preserve">93622</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC93622</t>
+  </si>
+  <si>
+    <t xml:space="preserve">115648</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC115648</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">285074</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC285074</t>
   </si>
   <si>
     <t xml:space="preserve">2</t>
   </si>
   <si>
-    <t xml:space="preserve">C12orf63</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GUSBP4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC387820</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC392395</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LINC00999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RASA4CP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RPS2P8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC441956</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21</t>
+    <t xml:space="preserve">286526</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAR2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">389833</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC389833</t>
+  </si>
+  <si>
+    <t xml:space="preserve">389834</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC389834</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un</t>
+  </si>
+  <si>
+    <t xml:space="preserve">400464</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC400464</t>
+  </si>
+  <si>
+    <t xml:space="preserve">400968</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC400968</t>
+  </si>
+  <si>
+    <t xml:space="preserve">401252</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC401252</t>
+  </si>
+  <si>
+    <t xml:space="preserve">440337</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC440337</t>
+  </si>
+  <si>
+    <t xml:space="preserve">440568</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC440568</t>
+  </si>
+  <si>
+    <t xml:space="preserve">441070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC441070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">441268</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC441268</t>
+  </si>
+  <si>
+    <t xml:space="preserve">442535</t>
   </si>
   <si>
     <t xml:space="preserve">LOC442535</t>
   </si>
   <si>
-    <t xml:space="preserve">PMS2P2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FAM45BP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPANXB2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SNHG3-RCC1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SYS1-DBNDD2</t>
+    <t xml:space="preserve">541469</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC541469</t>
+  </si>
+  <si>
+    <t xml:space="preserve">642897</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC642897</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90925</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC90925</t>
+  </si>
+  <si>
+    <t xml:space="preserve">143666</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC143666</t>
+  </si>
+  <si>
+    <t xml:space="preserve">284296</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC284296</t>
+  </si>
+  <si>
+    <t xml:space="preserve">400965</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC400965</t>
+  </si>
+  <si>
+    <t xml:space="preserve">401072</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC401072</t>
+  </si>
+  <si>
+    <t xml:space="preserve">402110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC402110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">439985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC439985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">440742</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC440742</t>
+  </si>
+  <si>
+    <t xml:space="preserve">613266</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC613266</t>
   </si>
   <si>
     <t xml:space="preserve">20</t>
   </si>
   <si>
-    <t xml:space="preserve">LINC00341</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BIN3-IT1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC90925</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC93622</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">115648</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC115648</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">155060</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC155060</t>
-  </si>
-  <si>
-    <t xml:space="preserve">283874</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC283874</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">285074</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC285074</t>
-  </si>
-  <si>
-    <t xml:space="preserve">286526</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RAR2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">339457</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C1orf222</t>
-  </si>
-  <si>
-    <t xml:space="preserve">387820</t>
-  </si>
-  <si>
-    <t xml:space="preserve">388022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC388022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">389833</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC389833</t>
-  </si>
-  <si>
-    <t xml:space="preserve">389834</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC389834</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Un</t>
-  </si>
-  <si>
-    <t xml:space="preserve">400464</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC400464</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">400499</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC400499</t>
-  </si>
-  <si>
-    <t xml:space="preserve">400924</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC400924</t>
-  </si>
-  <si>
-    <t xml:space="preserve">400968</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC400968</t>
-  </si>
-  <si>
-    <t xml:space="preserve">401252</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC401252</t>
-  </si>
-  <si>
-    <t xml:space="preserve">401589</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC401589</t>
-  </si>
-  <si>
-    <t xml:space="preserve">440337</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC440337</t>
-  </si>
-  <si>
-    <t xml:space="preserve">440568</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC440568</t>
-  </si>
-  <si>
-    <t xml:space="preserve">440570</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC440570</t>
-  </si>
-  <si>
-    <t xml:space="preserve">441070</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC441070</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">441120</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC441120</t>
-  </si>
-  <si>
-    <t xml:space="preserve">441193</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC441193</t>
-  </si>
-  <si>
-    <t xml:space="preserve">441257</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC441257</t>
-  </si>
-  <si>
-    <t xml:space="preserve">441268</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC441268</t>
-  </si>
-  <si>
-    <t xml:space="preserve">441956</t>
-  </si>
-  <si>
-    <t xml:space="preserve">442535</t>
-  </si>
-  <si>
-    <t xml:space="preserve">541469</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC541469</t>
-  </si>
-  <si>
-    <t xml:space="preserve">541473</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC541473</t>
-  </si>
-  <si>
-    <t xml:space="preserve">642897</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC642897</t>
-  </si>
-  <si>
-    <t xml:space="preserve">643576</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC643576</t>
-  </si>
-  <si>
-    <t xml:space="preserve">644563</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC644563</t>
-  </si>
-  <si>
-    <t xml:space="preserve">646347</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC646347</t>
-  </si>
-  <si>
-    <t xml:space="preserve">646517</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC646517</t>
-  </si>
-  <si>
-    <t xml:space="preserve">727726</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC727726</t>
-  </si>
-  <si>
-    <t xml:space="preserve">727849</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC727849</t>
-  </si>
-  <si>
-    <t xml:space="preserve">728392</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC728392</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">728454</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEFB4B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">88523</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC88523</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">90925</t>
-  </si>
-  <si>
-    <t xml:space="preserve">91431</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC91431</t>
-  </si>
-  <si>
-    <t xml:space="preserve">143188</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC143188</t>
-  </si>
-  <si>
-    <t xml:space="preserve">143666</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC143666</t>
-  </si>
-  <si>
-    <t xml:space="preserve">284009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC284009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">284296</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC284296</t>
-  </si>
-  <si>
-    <t xml:space="preserve">340843</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FAM23B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">387720</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC387720</t>
-  </si>
-  <si>
-    <t xml:space="preserve">387790</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC387790</t>
-  </si>
-  <si>
-    <t xml:space="preserve">392395</t>
-  </si>
-  <si>
-    <t xml:space="preserve">400965</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC400965</t>
-  </si>
-  <si>
-    <t xml:space="preserve">401052</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC401052</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">401072</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC401072</t>
-  </si>
-  <si>
-    <t xml:space="preserve">401410</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC401410</t>
-  </si>
-  <si>
-    <t xml:space="preserve">402110</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC402110</t>
-  </si>
-  <si>
-    <t xml:space="preserve">439985</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC439985</t>
-  </si>
-  <si>
-    <t xml:space="preserve">440742</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC440742</t>
-  </si>
-  <si>
-    <t xml:space="preserve">441233</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC441233</t>
-  </si>
-  <si>
-    <t xml:space="preserve">613266</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC613266</t>
-  </si>
-  <si>
-    <t xml:space="preserve">646434</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC646434</t>
-  </si>
-  <si>
     <t xml:space="preserve">647115</t>
   </si>
   <si>
     <t xml:space="preserve">LOC647115</t>
   </si>
   <si>
-    <t xml:space="preserve">727797</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC727797</t>
-  </si>
-  <si>
-    <t xml:space="preserve">729021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC729021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">93622</t>
-  </si>
-  <si>
-    <t xml:space="preserve">158318</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FAM27E1</t>
-  </si>
-  <si>
     <t xml:space="preserve">284912</t>
   </si>
   <si>
@@ -545,30 +554,12 @@
     <t xml:space="preserve">LOC399900</t>
   </si>
   <si>
-    <t xml:space="preserve">401296</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LNCRI</t>
-  </si>
-  <si>
     <t xml:space="preserve">401357</t>
   </si>
   <si>
     <t xml:space="preserve">LOC401357</t>
   </si>
   <si>
-    <t xml:space="preserve">401433</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC401433</t>
-  </si>
-  <si>
-    <t xml:space="preserve">401620</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOC401620</t>
-  </si>
-  <si>
     <t xml:space="preserve">440258</t>
   </si>
   <si>
@@ -579,12 +570,6 @@
   </si>
   <si>
     <t xml:space="preserve">FAM27E2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">653365</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASAH2C</t>
   </si>
   <si>
     <t xml:space="preserve">94431</t>
@@ -638,8 +623,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:D22" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:D22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:D48" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:D48"/>
   <tableColumns count="4">
     <tableColumn id="1" name="uid"/>
     <tableColumn id="2" name="name"/>
@@ -989,280 +974,624 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>100008589</v>
+      <c r="A2" t="s">
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2"/>
+        <v>6</v>
+      </c>
+      <c r="D2" t="n">
+        <v>114.610672</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>10748</v>
+      <c r="A3" t="s">
+        <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="n">
+        <v>149.28528</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2.65115</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2.40698</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="n">
-        <v>10.588477</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>130029</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D8" t="n">
+        <v>18.081223</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="n">
+        <v>127.734609</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="n">
+        <v>127.940983</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="n">
+        <v>104.719759</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" t="n">
+        <v>11.372014</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" t="n">
+        <v>10.006417</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="n">
-        <v>203.559077</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>374467</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>375513</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D17" t="n">
+        <v>1.690811</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" t="n">
+        <v>151.07413</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" t="n">
+        <v>52.05117</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" t="n">
+        <v>167.795528</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" t="n">
+        <v>5.426139</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" t="n">
+        <v>57.475796</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" t="n">
+        <v>13.679218</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" t="n">
+        <v>75.391948</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" t="n">
+        <v>104.030728</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" t="n">
+        <v>107.131573</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>83</v>
+      </c>
+      <c r="B34" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" t="n">
+        <v>160.894888</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" t="n">
+        <v>51.409883</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>89</v>
+      </c>
+      <c r="B37" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" t="n">
+        <v>50.187239</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" t="s">
+        <v>92</v>
+      </c>
+      <c r="C38" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="n">
-        <v>57.908552</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>387820</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="n">
-        <v>127.940983</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>392395</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>399744</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D38" t="n">
+        <v>39.443813</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" t="n">
+        <v>50.69633</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>95</v>
+      </c>
+      <c r="B40" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" t="s">
+        <v>43</v>
+      </c>
+      <c r="D40"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>97</v>
+      </c>
+      <c r="B41" t="s">
+        <v>98</v>
+      </c>
+      <c r="C41" t="s">
+        <v>99</v>
+      </c>
+      <c r="D41"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>100</v>
+      </c>
+      <c r="B42" t="s">
+        <v>101</v>
+      </c>
+      <c r="C42" t="s">
         <v>18</v>
       </c>
-      <c r="D9" t="n">
-        <v>38.428145</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>401331</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" t="n">
-        <v>44.028886</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>440589</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" t="n">
-        <v>51.250561</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>441956</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" t="n">
-        <v>13.679218</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>442535</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>5380</v>
-      </c>
-      <c r="B14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" t="n">
-        <v>75.343936</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>55855</v>
-      </c>
-      <c r="B15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" t="n">
-        <v>130.49494</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>64694</v>
-      </c>
-      <c r="B16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>751867</v>
-      </c>
-      <c r="B17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17"/>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>767557</v>
-      </c>
-      <c r="B18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" t="n">
-        <v>45.363168</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>79686</v>
-      </c>
-      <c r="B19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19"/>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>80094</v>
-      </c>
-      <c r="B20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" t="n">
-        <v>22.64037</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>90925</v>
-      </c>
-      <c r="B21" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21"/>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>93622</v>
-      </c>
-      <c r="B22" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" t="n">
+      <c r="D42" t="n">
+        <v>5.499426</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>102</v>
+      </c>
+      <c r="B43" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" t="n">
+        <v>7.259787</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>105</v>
+      </c>
+      <c r="B44" t="s">
+        <v>106</v>
+      </c>
+      <c r="C44" t="s">
+        <v>61</v>
+      </c>
+      <c r="D44" t="n">
+        <v>177.87526</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>107</v>
+      </c>
+      <c r="B45" t="s">
+        <v>108</v>
+      </c>
+      <c r="C45" t="s">
+        <v>109</v>
+      </c>
+      <c r="D45"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>110</v>
+      </c>
+      <c r="B46" t="s">
+        <v>111</v>
+      </c>
+      <c r="C46" t="s">
+        <v>112</v>
+      </c>
+      <c r="D46"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>113</v>
+      </c>
+      <c r="B47" t="s">
+        <v>114</v>
+      </c>
+      <c r="C47" t="s">
+        <v>109</v>
+      </c>
+      <c r="D47"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>115</v>
+      </c>
+      <c r="B48" t="s">
+        <v>116</v>
+      </c>
+      <c r="C48" t="s">
+        <v>109</v>
+      </c>
+      <c r="D48" t="n">
         <v>6.674093</v>
       </c>
     </row>
@@ -1299,25 +1628,25 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>119</v>
       </c>
       <c r="D2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D3" t="n">
         <v>149.28528</v>
@@ -1325,13 +1654,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="D4" t="n">
         <v>2.65115</v>
@@ -1339,13 +1668,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>120</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>121</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>122</v>
       </c>
       <c r="D5" t="n">
         <v>87.030674</v>
@@ -1353,37 +1682,37 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>123</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>124</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D8" t="n">
         <v>127.940983</v>
@@ -1391,13 +1720,13 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" t="n">
         <v>104.719759</v>
@@ -1405,37 +1734,37 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>125</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>126</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="D10"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>127</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>128</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>129</v>
       </c>
       <c r="D11"/>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>130</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>131</v>
       </c>
       <c r="C12" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="D12" t="n">
         <v>99.807022</v>
@@ -1443,13 +1772,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="D13" t="n">
         <v>11.372014</v>
@@ -1457,25 +1786,25 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="D14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>69</v>
+        <v>132</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>133</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="D15" t="n">
         <v>19.62067</v>
@@ -1483,13 +1812,13 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>134</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>135</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="D16" t="n">
         <v>32.331465</v>
@@ -1497,13 +1826,13 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D17" t="n">
         <v>52.05117</v>
@@ -1511,13 +1840,13 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>136</v>
       </c>
       <c r="B18" t="s">
-        <v>76</v>
+        <v>137</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="D18" t="n">
         <v>6.377742</v>
@@ -1525,13 +1854,13 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>77</v>
+        <v>138</v>
       </c>
       <c r="B19" t="s">
-        <v>78</v>
+        <v>139</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D19" t="n">
         <v>16.034509</v>
@@ -1539,25 +1868,25 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D20"/>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>81</v>
+        <v>140</v>
       </c>
       <c r="B21" t="s">
-        <v>82</v>
+        <v>141</v>
       </c>
       <c r="C21" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D21" t="n">
         <v>44.874939</v>
@@ -1565,25 +1894,25 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="C22" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D22"/>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D23" t="n">
         <v>5.426139</v>
@@ -1591,37 +1920,37 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="C24" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D24"/>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>90</v>
+        <v>142</v>
       </c>
       <c r="B25" t="s">
-        <v>91</v>
+        <v>143</v>
       </c>
       <c r="C25" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D25"/>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="C26" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="D26" t="n">
         <v>13.679218</v>
@@ -1629,37 +1958,37 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>93</v>
+        <v>144</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>145</v>
       </c>
       <c r="C27" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D27"/>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>146</v>
       </c>
       <c r="B28" t="s">
-        <v>95</v>
+        <v>147</v>
       </c>
       <c r="C28" t="s">
-        <v>42</v>
+        <v>119</v>
       </c>
       <c r="D28"/>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="B29" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="C29" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D29" t="n">
         <v>75.391948</v>
@@ -1667,13 +1996,13 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>98</v>
+        <v>148</v>
       </c>
       <c r="B30" t="s">
-        <v>99</v>
+        <v>149</v>
       </c>
       <c r="C30" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D30" t="n">
         <v>93.609431</v>
@@ -1681,13 +2010,13 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="B31" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>7</v>
+        <v>80</v>
       </c>
       <c r="D31" t="n">
         <v>104.030728</v>
@@ -1695,13 +2024,13 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="B32" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="C32" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D32" t="n">
         <v>107.131573</v>
@@ -1709,13 +2038,13 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="B33" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="C33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D33" t="n">
         <v>160.894888</v>
@@ -1723,13 +2052,13 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="B34" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="C34" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="D34" t="n">
         <v>51.409883</v>
@@ -1737,13 +2066,13 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="B35" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="C35" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D35" t="n">
         <v>50.69633</v>
@@ -1751,25 +2080,25 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="B36" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C36" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="D36"/>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B37" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C37" t="s">
-        <v>114</v>
+        <v>18</v>
       </c>
       <c r="D37" t="n">
         <v>5.499426</v>
@@ -1777,13 +2106,13 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="B38" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C38" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="D38" t="n">
         <v>7.259787</v>
@@ -1791,37 +2120,37 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B39" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C39" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D39"/>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="B40" t="s">
-        <v>37</v>
+        <v>151</v>
       </c>
       <c r="C40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D40"/>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B41" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C41" t="s">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="D41"/>
     </row>
@@ -1858,25 +2187,25 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>119</v>
       </c>
       <c r="D2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>124</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D3" t="n">
         <v>114.610672</v>
@@ -1884,13 +2213,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>152</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>153</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D4" t="n">
         <v>0.573807</v>
@@ -1898,13 +2227,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="D5" t="n">
         <v>2.65115</v>
@@ -1912,13 +2241,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>114</v>
+        <v>18</v>
       </c>
       <c r="D6" t="n">
         <v>2.40698</v>
@@ -1926,25 +2255,25 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
       <c r="B7" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>119</v>
       </c>
       <c r="D7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>120</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>121</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>122</v>
       </c>
       <c r="D8" t="n">
         <v>87.030674</v>
@@ -1952,25 +2281,25 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>123</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>124</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D9"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>132</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D10" t="n">
         <v>18.081223</v>
@@ -1978,13 +2307,13 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>133</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>134</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D11" t="n">
         <v>127.734609</v>
@@ -1992,25 +2321,25 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>135</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>136</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D12"/>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D13" t="n">
         <v>127.940983</v>
@@ -2018,13 +2347,13 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" t="n">
         <v>104.719759</v>
@@ -2032,37 +2361,37 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>125</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>126</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="D15"/>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>137</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D16"/>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>130</v>
       </c>
       <c r="B17" t="s">
-        <v>63</v>
+        <v>131</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="D17" t="n">
         <v>99.807022</v>
@@ -2070,13 +2399,13 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="D18" t="n">
         <v>11.372014</v>
@@ -2084,25 +2413,25 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="D19"/>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
       <c r="B20" t="s">
-        <v>139</v>
+        <v>157</v>
       </c>
       <c r="C20" t="s">
-        <v>9</v>
+        <v>122</v>
       </c>
       <c r="D20" t="n">
         <v>87.052748</v>
@@ -2110,13 +2439,13 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>140</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>141</v>
+        <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>142</v>
+        <v>43</v>
       </c>
       <c r="D21" t="n">
         <v>10.006417</v>
@@ -2124,13 +2453,13 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
       <c r="B22" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="C22" t="s">
-        <v>142</v>
+        <v>43</v>
       </c>
       <c r="D22" t="n">
         <v>70.745438</v>
@@ -2138,25 +2467,25 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>145</v>
+        <v>46</v>
       </c>
       <c r="B23" t="s">
-        <v>146</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D23"/>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D24" t="n">
         <v>52.05117</v>
@@ -2164,13 +2493,13 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="B25" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="C25" t="s">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="D25" t="n">
         <v>48.992527</v>
@@ -2178,13 +2507,13 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="B26" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C26" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D26" t="n">
         <v>76.825429</v>
@@ -2192,13 +2521,13 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>136</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>137</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="D27" t="n">
         <v>6.377742</v>
@@ -2206,13 +2535,13 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>77</v>
+        <v>138</v>
       </c>
       <c r="B28" t="s">
-        <v>78</v>
+        <v>139</v>
       </c>
       <c r="C28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D28" t="n">
         <v>16.034509</v>
@@ -2220,25 +2549,25 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="B29" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="C29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D29"/>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="B30" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="C30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D30" t="n">
         <v>244.064329</v>
@@ -2246,25 +2575,25 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="B31" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="C31" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>153</v>
+        <v>69</v>
       </c>
       <c r="B32" t="s">
-        <v>154</v>
+        <v>70</v>
       </c>
       <c r="C32" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D32" t="n">
         <v>57.475796</v>
@@ -2272,37 +2601,37 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="B33" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="C33" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D33"/>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>90</v>
+        <v>142</v>
       </c>
       <c r="B34" t="s">
-        <v>91</v>
+        <v>143</v>
       </c>
       <c r="C34" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D34"/>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="B35" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="C35" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="D35" t="n">
         <v>13.679218</v>
@@ -2310,25 +2639,25 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>94</v>
+        <v>146</v>
       </c>
       <c r="B36" t="s">
-        <v>95</v>
+        <v>147</v>
       </c>
       <c r="C36" t="s">
-        <v>42</v>
+        <v>119</v>
       </c>
       <c r="D36"/>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="B37" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="C37" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D37" t="n">
         <v>75.391948</v>
@@ -2336,13 +2665,13 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="B38" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="C38" t="s">
-        <v>32</v>
+        <v>168</v>
       </c>
       <c r="D38" t="n">
         <v>15.892332</v>
@@ -2350,13 +2679,13 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="B39" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="C39" t="s">
-        <v>7</v>
+        <v>80</v>
       </c>
       <c r="D39" t="n">
         <v>104.030728</v>
@@ -2364,13 +2693,13 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="B40" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="C40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D40" t="n">
         <v>160.894888</v>
@@ -2378,25 +2707,25 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>157</v>
+        <v>85</v>
       </c>
       <c r="B41" t="s">
-        <v>158</v>
+        <v>86</v>
       </c>
       <c r="C41" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D41"/>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="B42" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="C42" t="s">
-        <v>9</v>
+        <v>122</v>
       </c>
       <c r="D42" t="n">
         <v>63.841106</v>
@@ -2404,13 +2733,13 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="B43" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="C43" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D43" t="n">
         <v>50.69633</v>
@@ -2418,73 +2747,73 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>161</v>
+        <v>95</v>
       </c>
       <c r="B44" t="s">
-        <v>162</v>
+        <v>96</v>
       </c>
       <c r="C44" t="s">
-        <v>142</v>
+        <v>43</v>
       </c>
       <c r="D44"/>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="B45" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C45" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="D45"/>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>163</v>
+        <v>107</v>
       </c>
       <c r="B46" t="s">
-        <v>164</v>
+        <v>108</v>
       </c>
       <c r="C46" t="s">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="D46"/>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B47" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C47" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D47"/>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B48" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C48" t="s">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="D48"/>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>165</v>
+        <v>115</v>
       </c>
       <c r="B49" t="s">
-        <v>38</v>
+        <v>116</v>
       </c>
       <c r="C49" t="s">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="D49" t="n">
         <v>6.674093</v>
@@ -2523,25 +2852,25 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>119</v>
       </c>
       <c r="D2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>124</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D3" t="n">
         <v>114.610672</v>
@@ -2549,13 +2878,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>152</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>153</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D4" t="n">
         <v>0.573807</v>
@@ -2563,13 +2892,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D5" t="n">
         <v>149.28528</v>
@@ -2577,25 +2906,25 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>166</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>167</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="D7" t="n">
         <v>2.65115</v>
@@ -2603,13 +2932,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B8" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="D8" t="n">
         <v>35.627575</v>
@@ -2617,37 +2946,37 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>123</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>124</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D9"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D11" t="n">
         <v>127.940983</v>
@@ -2655,13 +2984,13 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B12" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="D12" t="n">
         <v>7.939</v>
@@ -2669,13 +2998,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B13" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D13" t="n">
         <v>72.490259</v>
@@ -2683,37 +3012,37 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>125</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>126</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="D14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>137</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D15"/>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B16" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C16" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D16" t="n">
         <v>61.967797</v>
@@ -2721,13 +3050,13 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="D17" t="n">
         <v>11.372014</v>
@@ -2735,13 +3064,13 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
       <c r="B18" t="s">
-        <v>139</v>
+        <v>157</v>
       </c>
       <c r="C18" t="s">
-        <v>9</v>
+        <v>122</v>
       </c>
       <c r="D18" t="n">
         <v>87.052748</v>
@@ -2749,13 +3078,13 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>140</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>141</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>142</v>
+        <v>43</v>
       </c>
       <c r="D19" t="n">
         <v>10.006417</v>
@@ -2763,13 +3092,13 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>134</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>135</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="D20" t="n">
         <v>32.331465</v>
@@ -2777,13 +3106,13 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>176</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>177</v>
+        <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D21" t="n">
         <v>1.690811</v>
@@ -2791,13 +3120,13 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B22" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D22" t="n">
         <v>56.809123</v>
@@ -2805,13 +3134,13 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>180</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>181</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D23" t="n">
         <v>151.07413</v>
@@ -2819,37 +3148,37 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>182</v>
+        <v>53</v>
       </c>
       <c r="B24" t="s">
-        <v>183</v>
+        <v>54</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D24"/>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B25" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="D25"/>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>136</v>
       </c>
       <c r="B26" t="s">
-        <v>76</v>
+        <v>137</v>
       </c>
       <c r="C26" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="D26" t="n">
         <v>6.377742</v>
@@ -2857,13 +3186,13 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>138</v>
       </c>
       <c r="B27" t="s">
-        <v>78</v>
+        <v>139</v>
       </c>
       <c r="C27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D27" t="n">
         <v>16.034509</v>
@@ -2871,37 +3200,37 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="B28" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="C28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D28"/>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="C29" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D29"/>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="B30" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="C30" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D30" t="n">
         <v>5.426139</v>
@@ -2909,25 +3238,25 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="B31" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="C31" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="B32" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="C32" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="D32" t="n">
         <v>13.679218</v>
@@ -2935,25 +3264,25 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B33" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C33" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D33"/>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="B34" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="C34" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D34" t="n">
         <v>75.391948</v>
@@ -2961,13 +3290,13 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="B35" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="C35" t="s">
-        <v>32</v>
+        <v>168</v>
       </c>
       <c r="D35" t="n">
         <v>15.892332</v>
@@ -2975,13 +3304,13 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="B36" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="C36" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D36" t="n">
         <v>107.131573</v>
@@ -2989,13 +3318,13 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="B37" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="C37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D37" t="n">
         <v>160.894888</v>
@@ -3003,25 +3332,25 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>157</v>
+        <v>85</v>
       </c>
       <c r="B38" t="s">
-        <v>158</v>
+        <v>86</v>
       </c>
       <c r="C38" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D38"/>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="B39" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="C39" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="D39" t="n">
         <v>51.409883</v>
@@ -3029,13 +3358,13 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="B40" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="C40" t="s">
-        <v>9</v>
+        <v>122</v>
       </c>
       <c r="D40" t="n">
         <v>63.841106</v>
@@ -3043,13 +3372,13 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>188</v>
+        <v>89</v>
       </c>
       <c r="B41" t="s">
-        <v>189</v>
+        <v>90</v>
       </c>
       <c r="C41" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D41" t="n">
         <v>50.187239</v>
@@ -3057,13 +3386,13 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="B42" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="C42" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D42" t="n">
         <v>50.69633</v>
@@ -3071,37 +3400,37 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>161</v>
+        <v>95</v>
       </c>
       <c r="B43" t="s">
-        <v>162</v>
+        <v>96</v>
       </c>
       <c r="C43" t="s">
-        <v>142</v>
+        <v>43</v>
       </c>
       <c r="D43"/>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="B44" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C44" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="D44"/>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B45" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C45" t="s">
-        <v>114</v>
+        <v>18</v>
       </c>
       <c r="D45" t="n">
         <v>5.499426</v>
@@ -3109,13 +3438,13 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="B46" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C46" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="D46" t="n">
         <v>7.259787</v>
@@ -3123,25 +3452,25 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="B47" t="s">
-        <v>37</v>
+        <v>151</v>
       </c>
       <c r="C47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D47"/>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B48" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C48" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="D48" t="n">
         <v>21.715451</v>

</xml_diff>